<commit_message>
Fixed contribution count error
</commit_message>
<xml_diff>
--- a/docs/Commits.xlsx
+++ b/docs/Commits.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PHPStorm\COM6504-Assignment\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E7BD302-C45C-462D-BEAC-DCDCA2A1E540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F04745-31D5-4FF6-8DCD-3427A967B4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB05932A-6599-4E74-8602-71EFDE2B9654}"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2206,13 +2219,13 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2223,12 +2236,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2260,10 +2267,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2313,6 +2320,12 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2700,8 +2713,8 @@
   </sheetPr>
   <dimension ref="B1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection sqref="A1:H170"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,75 +2731,75 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>490</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="33" t="s">
         <v>495</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="34" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>497</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="22">
         <f>COUNTIF(B9:B169,B3)</f>
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>498</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>500</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="26">
         <f t="shared" ref="E4:E6" si="0">COUNTIF(B10:B170,B4)</f>
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="E5" s="28">
-        <f t="shared" si="0"/>
-        <v>7</v>
+      <c r="E5" s="26">
+        <f>COUNTIF(B9:B169,B5) + COUNTIF(B9:B169, "Koustav Muhuri")</f>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="29" t="s">
         <v>502</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2802,20 +2815,20 @@
       <c r="D8" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="35" t="s">
         <v>493</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2824,18 +2837,18 @@
       <c r="F9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2844,18 +2857,18 @@
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2864,16 +2877,16 @@
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2882,18 +2895,18 @@
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2902,18 +2915,18 @@
       <c r="F13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2922,18 +2935,18 @@
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -2942,18 +2955,18 @@
       <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2962,16 +2975,16 @@
       <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2980,18 +2993,18 @@
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="15" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -3000,18 +3013,18 @@
       <c r="F18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="17" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -3020,18 +3033,18 @@
       <c r="F19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="15" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -3040,18 +3053,18 @@
       <c r="F20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -3060,18 +3073,18 @@
       <c r="F21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="15" t="s">
         <v>61</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -3080,16 +3093,16 @@
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -3098,18 +3111,18 @@
       <c r="F23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -3118,18 +3131,18 @@
       <c r="F24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="15" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -3138,16 +3151,16 @@
       <c r="F25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="19"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -3156,18 +3169,18 @@
       <c r="F26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="15" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -3176,18 +3189,18 @@
       <c r="F27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="15" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -3196,18 +3209,18 @@
       <c r="F28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="15" t="s">
         <v>84</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -3216,18 +3229,18 @@
       <c r="F29" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="15" t="s">
         <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -3236,18 +3249,18 @@
       <c r="F30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="15" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -3256,18 +3269,18 @@
       <c r="F31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="15" t="s">
         <v>95</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -3276,18 +3289,18 @@
       <c r="F32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="15" t="s">
         <v>99</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -3296,18 +3309,18 @@
       <c r="F33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="15" t="s">
         <v>103</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -3316,18 +3329,18 @@
       <c r="F34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="15" t="s">
         <v>105</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -3336,18 +3349,18 @@
       <c r="F35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="15" t="s">
         <v>109</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -3356,18 +3369,18 @@
       <c r="F36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="15" t="s">
         <v>114</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -3376,18 +3389,18 @@
       <c r="F37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="15" t="s">
         <v>117</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -3396,18 +3409,18 @@
       <c r="F38" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="15" t="s">
         <v>121</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -3416,16 +3429,16 @@
       <c r="F39" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="15" t="s">
         <v>124</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -3434,18 +3447,18 @@
       <c r="F40" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="12" t="s">
+      <c r="B41" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="15" t="s">
         <v>127</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -3454,18 +3467,18 @@
       <c r="F41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="17" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="15" t="s">
         <v>131</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -3474,18 +3487,18 @@
       <c r="F42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="17" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="12" t="s">
+      <c r="B43" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="15" t="s">
         <v>135</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -3494,18 +3507,18 @@
       <c r="F43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G43" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="B44" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="15" t="s">
         <v>138</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -3514,16 +3527,16 @@
       <c r="F44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G44" s="19"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="12" t="s">
+      <c r="B45" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="15" t="s">
         <v>141</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -3532,18 +3545,18 @@
       <c r="F45" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="17" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="12" t="s">
+      <c r="B46" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="15" t="s">
         <v>145</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3552,16 +3565,16 @@
       <c r="F46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G46" s="19"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="15" t="s">
         <v>148</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -3570,18 +3583,18 @@
       <c r="F47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="12" t="s">
+      <c r="B48" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="15" t="s">
         <v>150</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -3590,18 +3603,18 @@
       <c r="F48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="G48" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="12" t="s">
+      <c r="B49" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="15" t="s">
         <v>153</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -3610,18 +3623,18 @@
       <c r="F49" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G49" s="19" t="s">
+      <c r="G49" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="12" t="s">
+      <c r="B50" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="15" t="s">
         <v>157</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -3630,18 +3643,18 @@
       <c r="F50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="15" t="s">
         <v>161</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -3650,16 +3663,16 @@
       <c r="F51" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G51" s="19"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="15" t="s">
         <v>131</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -3668,18 +3681,18 @@
       <c r="F52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="G52" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="15" t="s">
         <v>164</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -3688,16 +3701,16 @@
       <c r="F53" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G53" s="19"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="15" t="s">
         <v>167</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -3706,18 +3719,18 @@
       <c r="F54" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="15" t="s">
         <v>170</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -3726,18 +3739,18 @@
       <c r="F55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="15" t="s">
         <v>173</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -3746,18 +3759,18 @@
       <c r="F56" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D57" s="17" t="s">
+      <c r="D57" s="15" t="s">
         <v>176</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -3766,16 +3779,16 @@
       <c r="F57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G57" s="19"/>
+      <c r="G57" s="17"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D58" s="15" t="s">
         <v>178</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -3784,18 +3797,18 @@
       <c r="F58" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="12" t="s">
+      <c r="B59" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="15" t="s">
         <v>181</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -3804,16 +3817,16 @@
       <c r="F59" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G59" s="19"/>
+      <c r="G59" s="17"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="12" t="s">
+      <c r="B60" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="15" t="s">
         <v>184</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -3822,18 +3835,18 @@
       <c r="F60" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="17" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="12" t="s">
+      <c r="B61" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="15" t="s">
         <v>187</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -3842,16 +3855,16 @@
       <c r="F61" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G61" s="19"/>
+      <c r="G61" s="17"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="15" t="s">
         <v>190</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -3860,18 +3873,18 @@
       <c r="F62" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="15" t="s">
         <v>192</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -3880,18 +3893,18 @@
       <c r="F63" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="12" t="s">
+      <c r="B64" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="15" t="s">
         <v>195</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -3900,18 +3913,18 @@
       <c r="F64" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="15" t="s">
         <v>199</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -3920,18 +3933,18 @@
       <c r="F65" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="15" t="s">
         <v>202</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -3940,18 +3953,18 @@
       <c r="F66" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="12" t="s">
+      <c r="B67" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="D67" s="15" t="s">
         <v>205</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -3960,18 +3973,18 @@
       <c r="F67" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="17" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="12" t="s">
+      <c r="B68" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D68" s="15" t="s">
         <v>209</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -3980,18 +3993,18 @@
       <c r="F68" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="G68" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B69" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="12" t="s">
+      <c r="B69" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D69" s="15" t="s">
         <v>211</v>
       </c>
       <c r="E69" s="1" t="s">
@@ -4000,18 +4013,18 @@
       <c r="F69" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G69" s="19" t="s">
+      <c r="G69" s="17" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="12" t="s">
+      <c r="B70" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="D70" s="15" t="s">
         <v>215</v>
       </c>
       <c r="E70" s="1" t="s">
@@ -4020,18 +4033,18 @@
       <c r="F70" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="12" t="s">
+      <c r="B71" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D71" s="15" t="s">
         <v>217</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -4040,18 +4053,18 @@
       <c r="F71" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G71" s="19" t="s">
+      <c r="G71" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D72" s="17" t="s">
+      <c r="D72" s="15" t="s">
         <v>220</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -4060,18 +4073,18 @@
       <c r="F72" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G72" s="19" t="s">
+      <c r="G72" s="17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D73" s="15" t="s">
         <v>223</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -4080,18 +4093,18 @@
       <c r="F73" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G73" s="19" t="s">
+      <c r="G73" s="17" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D74" s="15" t="s">
         <v>226</v>
       </c>
       <c r="E74" s="1" t="s">
@@ -4100,18 +4113,18 @@
       <c r="F74" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G74" s="19" t="s">
+      <c r="G74" s="17" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D75" s="17" t="s">
+      <c r="D75" s="15" t="s">
         <v>229</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -4120,18 +4133,18 @@
       <c r="F75" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G75" s="19" t="s">
+      <c r="G75" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D76" s="17" t="s">
+      <c r="D76" s="15" t="s">
         <v>233</v>
       </c>
       <c r="E76" s="1" t="s">
@@ -4140,18 +4153,18 @@
       <c r="F76" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G76" s="19" t="s">
+      <c r="G76" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D77" s="15" t="s">
         <v>238</v>
       </c>
       <c r="E77" s="1" t="s">
@@ -4160,16 +4173,16 @@
       <c r="F77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G77" s="19"/>
+      <c r="G77" s="17"/>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D78" s="17" t="s">
+      <c r="D78" s="15" t="s">
         <v>238</v>
       </c>
       <c r="E78" s="1" t="s">
@@ -4178,18 +4191,18 @@
       <c r="F78" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G78" s="19" t="s">
+      <c r="G78" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D79" s="17" t="s">
+      <c r="D79" s="15" t="s">
         <v>242</v>
       </c>
       <c r="E79" s="1" t="s">
@@ -4198,16 +4211,16 @@
       <c r="F79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G79" s="19"/>
+      <c r="G79" s="17"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C80" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D80" s="17" t="s">
+      <c r="D80" s="15" t="s">
         <v>244</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -4216,18 +4229,18 @@
       <c r="F80" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G80" s="19" t="s">
+      <c r="G80" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D81" s="17" t="s">
+      <c r="D81" s="15" t="s">
         <v>246</v>
       </c>
       <c r="E81" s="1" t="s">
@@ -4236,18 +4249,18 @@
       <c r="F81" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="19" t="s">
+      <c r="G81" s="17" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="12" t="s">
+      <c r="B82" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="D82" s="17" t="s">
+      <c r="D82" s="15" t="s">
         <v>250</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -4256,18 +4269,18 @@
       <c r="F82" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="G82" s="19" t="s">
+      <c r="G82" s="17" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="C83" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="15" t="s">
         <v>254</v>
       </c>
       <c r="E83" s="1" t="s">
@@ -4276,18 +4289,18 @@
       <c r="F83" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G83" s="19" t="s">
+      <c r="G83" s="17" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="84" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="C84" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="D84" s="17" t="s">
+      <c r="D84" s="15" t="s">
         <v>257</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -4296,18 +4309,18 @@
       <c r="F84" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G84" s="19" t="s">
+      <c r="G84" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="D85" s="17" t="s">
+      <c r="D85" s="15" t="s">
         <v>262</v>
       </c>
       <c r="E85" s="1" t="s">
@@ -4316,18 +4329,18 @@
       <c r="F85" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G85" s="19" t="s">
+      <c r="G85" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C86" s="12" t="s">
+      <c r="C86" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="D86" s="17" t="s">
+      <c r="D86" s="15" t="s">
         <v>262</v>
       </c>
       <c r="E86" s="1" t="s">
@@ -4336,18 +4349,18 @@
       <c r="F86" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G86" s="19" t="s">
+      <c r="G86" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C87" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="D87" s="17" t="s">
+      <c r="D87" s="15" t="s">
         <v>266</v>
       </c>
       <c r="E87" s="1" t="s">
@@ -4356,18 +4369,18 @@
       <c r="F87" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G87" s="19" t="s">
+      <c r="G87" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="12" t="s">
+      <c r="C88" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="D88" s="17" t="s">
+      <c r="D88" s="15" t="s">
         <v>268</v>
       </c>
       <c r="E88" s="1" t="s">
@@ -4376,18 +4389,18 @@
       <c r="F88" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G88" s="19" t="s">
+      <c r="G88" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C89" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="15" t="s">
         <v>270</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -4396,18 +4409,18 @@
       <c r="F89" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G89" s="19" t="s">
+      <c r="G89" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C90" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="D90" s="17" t="s">
+      <c r="D90" s="15" t="s">
         <v>274</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -4416,18 +4429,18 @@
       <c r="F90" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G90" s="19" t="s">
+      <c r="G90" s="17" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="C91" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="D91" s="17" t="s">
+      <c r="D91" s="15" t="s">
         <v>278</v>
       </c>
       <c r="E91" s="1" t="s">
@@ -4436,18 +4449,18 @@
       <c r="F91" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G91" s="19" t="s">
+      <c r="G91" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C92" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="15" t="s">
         <v>281</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -4456,18 +4469,18 @@
       <c r="F92" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G92" s="19" t="s">
+      <c r="G92" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="D93" s="17" t="s">
+      <c r="D93" s="15" t="s">
         <v>283</v>
       </c>
       <c r="E93" s="1" t="s">
@@ -4476,18 +4489,18 @@
       <c r="F93" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G93" s="19" t="s">
+      <c r="G93" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C94" s="12" t="s">
+      <c r="C94" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D94" s="17" t="s">
+      <c r="D94" s="15" t="s">
         <v>285</v>
       </c>
       <c r="E94" s="1" t="s">
@@ -4496,18 +4509,18 @@
       <c r="F94" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G94" s="19" t="s">
+      <c r="G94" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C95" s="12" t="s">
+      <c r="B95" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="D95" s="17" t="s">
+      <c r="D95" s="15" t="s">
         <v>288</v>
       </c>
       <c r="E95" s="1" t="s">
@@ -4516,18 +4529,18 @@
       <c r="F95" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G95" s="19" t="s">
+      <c r="G95" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C96" s="12" t="s">
+      <c r="B96" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D96" s="17" t="s">
+      <c r="D96" s="15" t="s">
         <v>290</v>
       </c>
       <c r="E96" s="1" t="s">
@@ -4536,18 +4549,18 @@
       <c r="F96" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G96" s="19" t="s">
+      <c r="G96" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C97" s="12" t="s">
+      <c r="B97" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="D97" s="17" t="s">
+      <c r="D97" s="15" t="s">
         <v>293</v>
       </c>
       <c r="E97" s="1" t="s">
@@ -4556,18 +4569,18 @@
       <c r="F97" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G97" s="19" t="s">
+      <c r="G97" s="17" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B98" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="12" t="s">
+      <c r="B98" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="D98" s="17" t="s">
+      <c r="D98" s="15" t="s">
         <v>295</v>
       </c>
       <c r="E98" s="1" t="s">
@@ -4576,18 +4589,18 @@
       <c r="F98" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G98" s="19" t="s">
+      <c r="G98" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="99" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C99" s="12" t="s">
+      <c r="B99" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="D99" s="17" t="s">
+      <c r="D99" s="15" t="s">
         <v>297</v>
       </c>
       <c r="E99" s="1" t="s">
@@ -4596,18 +4609,18 @@
       <c r="F99" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G99" s="19" t="s">
+      <c r="G99" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="12" t="s">
+      <c r="B100" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="D100" s="17" t="s">
+      <c r="D100" s="15" t="s">
         <v>300</v>
       </c>
       <c r="E100" s="1" t="s">
@@ -4616,16 +4629,16 @@
       <c r="F100" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G100" s="19"/>
+      <c r="G100" s="17"/>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C101" s="12" t="s">
+      <c r="C101" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="D101" s="17" t="s">
+      <c r="D101" s="15" t="s">
         <v>302</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -4634,18 +4647,18 @@
       <c r="F101" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G101" s="19" t="s">
+      <c r="G101" s="17" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="12" t="s">
+      <c r="B102" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D102" s="17" t="s">
+      <c r="D102" s="15" t="s">
         <v>305</v>
       </c>
       <c r="E102" s="1" t="s">
@@ -4654,18 +4667,18 @@
       <c r="F102" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G102" s="19" t="s">
+      <c r="G102" s="17" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C103" s="12" t="s">
+      <c r="B103" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="D103" s="17" t="s">
+      <c r="D103" s="15" t="s">
         <v>309</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -4674,18 +4687,18 @@
       <c r="F103" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G103" s="19" t="s">
+      <c r="G103" s="17" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C104" s="12" t="s">
+      <c r="B104" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="D104" s="17" t="s">
+      <c r="D104" s="15" t="s">
         <v>313</v>
       </c>
       <c r="E104" s="1" t="s">
@@ -4694,18 +4707,18 @@
       <c r="F104" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G104" s="19" t="s">
+      <c r="G104" s="17" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="12" t="s">
+      <c r="B105" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="D105" s="17" t="s">
+      <c r="D105" s="15" t="s">
         <v>317</v>
       </c>
       <c r="E105" s="1" t="s">
@@ -4714,16 +4727,16 @@
       <c r="F105" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G105" s="19"/>
+      <c r="G105" s="17"/>
     </row>
     <row r="106" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B106" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="12" t="s">
+      <c r="B106" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="D106" s="17" t="s">
+      <c r="D106" s="15" t="s">
         <v>320</v>
       </c>
       <c r="E106" s="1" t="s">
@@ -4732,18 +4745,18 @@
       <c r="F106" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="G106" s="19" t="s">
+      <c r="G106" s="17" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C107" s="12" t="s">
+      <c r="B107" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="D107" s="17" t="s">
+      <c r="D107" s="15" t="s">
         <v>325</v>
       </c>
       <c r="E107" s="1" t="s">
@@ -4752,18 +4765,18 @@
       <c r="F107" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="G107" s="19" t="s">
+      <c r="G107" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C108" s="12" t="s">
+      <c r="B108" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="D108" s="17" t="s">
+      <c r="D108" s="15" t="s">
         <v>328</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -4772,18 +4785,18 @@
       <c r="F108" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G108" s="19" t="s">
+      <c r="G108" s="17" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C109" s="12" t="s">
+      <c r="B109" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="D109" s="17" t="s">
+      <c r="D109" s="15" t="s">
         <v>331</v>
       </c>
       <c r="E109" s="1" t="s">
@@ -4792,18 +4805,18 @@
       <c r="F109" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G109" s="19" t="s">
+      <c r="G109" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C110" s="12" t="s">
+      <c r="B110" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="D110" s="17" t="s">
+      <c r="D110" s="15" t="s">
         <v>333</v>
       </c>
       <c r="E110" s="1" t="s">
@@ -4812,18 +4825,18 @@
       <c r="F110" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="G110" s="19" t="s">
+      <c r="G110" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C111" s="12" t="s">
+      <c r="B111" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="D111" s="17" t="s">
+      <c r="D111" s="15" t="s">
         <v>336</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -4832,18 +4845,18 @@
       <c r="F111" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="G111" s="19" t="s">
+      <c r="G111" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C112" s="12" t="s">
+      <c r="B112" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="D112" s="17" t="s">
+      <c r="D112" s="15" t="s">
         <v>339</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -4852,18 +4865,18 @@
       <c r="F112" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G112" s="19" t="s">
+      <c r="G112" s="17" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B113" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C113" s="12" t="s">
+      <c r="B113" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="D113" s="17" t="s">
+      <c r="D113" s="15" t="s">
         <v>343</v>
       </c>
       <c r="E113" s="1" t="s">
@@ -4872,18 +4885,18 @@
       <c r="F113" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G113" s="19" t="s">
+      <c r="G113" s="17" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C114" s="12" t="s">
+      <c r="B114" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="D114" s="17" t="s">
+      <c r="D114" s="15" t="s">
         <v>346</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -4892,18 +4905,18 @@
       <c r="F114" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="G114" s="19" t="s">
+      <c r="G114" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B115" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C115" s="12" t="s">
+      <c r="B115" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="D115" s="17" t="s">
+      <c r="D115" s="15" t="s">
         <v>349</v>
       </c>
       <c r="E115" s="1" t="s">
@@ -4912,18 +4925,18 @@
       <c r="F115" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="G115" s="19" t="s">
+      <c r="G115" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C116" s="12" t="s">
+      <c r="B116" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="D116" s="17" t="s">
+      <c r="D116" s="15" t="s">
         <v>352</v>
       </c>
       <c r="E116" s="1" t="s">
@@ -4932,18 +4945,18 @@
       <c r="F116" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G116" s="19" t="s">
+      <c r="G116" s="17" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C117" s="12" t="s">
+      <c r="C117" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D117" s="17" t="s">
+      <c r="D117" s="15" t="s">
         <v>356</v>
       </c>
       <c r="E117" s="1" t="s">
@@ -4952,18 +4965,18 @@
       <c r="F117" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G117" s="19" t="s">
+      <c r="G117" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C118" s="12" t="s">
+      <c r="C118" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="D118" s="17" t="s">
+      <c r="D118" s="15" t="s">
         <v>358</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -4972,18 +4985,18 @@
       <c r="F118" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G118" s="19" t="s">
+      <c r="G118" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C119" s="12" t="s">
+      <c r="C119" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="D119" s="17" t="s">
+      <c r="D119" s="15" t="s">
         <v>360</v>
       </c>
       <c r="E119" s="1" t="s">
@@ -4992,18 +5005,18 @@
       <c r="F119" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="G119" s="19" t="s">
+      <c r="G119" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C120" s="12" t="s">
+      <c r="B120" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="D120" s="17" t="s">
+      <c r="D120" s="15" t="s">
         <v>363</v>
       </c>
       <c r="E120" s="1" t="s">
@@ -5012,18 +5025,18 @@
       <c r="F120" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G120" s="19" t="s">
+      <c r="G120" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C121" s="12" t="s">
+      <c r="B121" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="D121" s="17" t="s">
+      <c r="D121" s="15" t="s">
         <v>366</v>
       </c>
       <c r="E121" s="1" t="s">
@@ -5032,18 +5045,18 @@
       <c r="F121" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="G121" s="19" t="s">
+      <c r="G121" s="17" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="11" t="s">
+      <c r="B122" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C122" s="12" t="s">
+      <c r="C122" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="D122" s="17" t="s">
+      <c r="D122" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -5052,18 +5065,18 @@
       <c r="F122" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G122" s="19" t="s">
+      <c r="G122" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C123" s="12" t="s">
+      <c r="C123" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="D123" s="17" t="s">
+      <c r="D123" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E123" s="1" t="s">
@@ -5072,18 +5085,18 @@
       <c r="F123" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G123" s="19" t="s">
+      <c r="G123" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C124" s="12" t="s">
+      <c r="C124" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D124" s="15" t="s">
         <v>373</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -5092,18 +5105,18 @@
       <c r="F124" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G124" s="19" t="s">
+      <c r="G124" s="17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C125" s="12" t="s">
+      <c r="B125" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="D125" s="17" t="s">
+      <c r="D125" s="15" t="s">
         <v>375</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -5112,18 +5125,18 @@
       <c r="F125" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G125" s="19" t="s">
+      <c r="G125" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C126" s="12" t="s">
+      <c r="B126" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="D126" s="17" t="s">
+      <c r="D126" s="15" t="s">
         <v>377</v>
       </c>
       <c r="E126" s="1" t="s">
@@ -5132,18 +5145,18 @@
       <c r="F126" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="G126" s="19" t="s">
+      <c r="G126" s="17" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C127" s="12" t="s">
+      <c r="B127" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="D127" s="17" t="s">
+      <c r="D127" s="15" t="s">
         <v>381</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -5152,18 +5165,18 @@
       <c r="F127" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="G127" s="19" t="s">
+      <c r="G127" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C128" s="12" t="s">
+      <c r="C128" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="D128" s="17">
+      <c r="D128" s="15">
         <v>12</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -5172,18 +5185,18 @@
       <c r="F128" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="G128" s="19" t="s">
+      <c r="G128" s="17" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B129" s="11" t="s">
+      <c r="B129" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C129" s="12" t="s">
+      <c r="C129" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="D129" s="17" t="s">
+      <c r="D129" s="15" t="s">
         <v>356</v>
       </c>
       <c r="E129" s="1" t="s">
@@ -5192,18 +5205,18 @@
       <c r="F129" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G129" s="19" t="s">
+      <c r="G129" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130" s="11" t="s">
+      <c r="B130" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C130" s="12" t="s">
+      <c r="C130" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="D130" s="17" t="s">
+      <c r="D130" s="15" t="s">
         <v>387</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -5212,16 +5225,16 @@
       <c r="F130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G130" s="19"/>
+      <c r="G130" s="17"/>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B131" s="11" t="s">
+      <c r="B131" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C131" s="12" t="s">
+      <c r="C131" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="D131" s="17" t="s">
+      <c r="D131" s="15" t="s">
         <v>389</v>
       </c>
       <c r="E131" s="1" t="s">
@@ -5230,18 +5243,18 @@
       <c r="F131" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="G131" s="19" t="s">
+      <c r="G131" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B132" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="B132" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="D132" s="17" t="s">
+      <c r="D132" s="15" t="s">
         <v>393</v>
       </c>
       <c r="E132" s="1" t="s">
@@ -5250,16 +5263,16 @@
       <c r="F132" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G132" s="19"/>
+      <c r="G132" s="17"/>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B133" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C133" s="12" t="s">
+      <c r="B133" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="D133" s="17" t="s">
+      <c r="D133" s="15" t="s">
         <v>393</v>
       </c>
       <c r="E133" s="1" t="s">
@@ -5268,18 +5281,18 @@
       <c r="F133" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G133" s="19" t="s">
+      <c r="G133" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="11" t="s">
+      <c r="B134" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="C134" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="D134" s="17" t="s">
+      <c r="D134" s="15" t="s">
         <v>396</v>
       </c>
       <c r="E134" s="1" t="s">
@@ -5288,18 +5301,18 @@
       <c r="F134" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G134" s="19" t="s">
+      <c r="G134" s="17" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B135" s="11" t="s">
+      <c r="B135" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C135" s="12" t="s">
+      <c r="C135" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="D135" s="17" t="s">
+      <c r="D135" s="15" t="s">
         <v>399</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -5308,18 +5321,18 @@
       <c r="F135" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G135" s="19" t="s">
+      <c r="G135" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="136" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B136" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C136" s="12" t="s">
+      <c r="B136" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="D136" s="17" t="s">
+      <c r="D136" s="15" t="s">
         <v>402</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -5328,18 +5341,18 @@
       <c r="F136" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G136" s="19" t="s">
+      <c r="G136" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C137" s="12" t="s">
+      <c r="C137" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="D137" s="17" t="s">
+      <c r="D137" s="15" t="s">
         <v>405</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -5348,18 +5361,18 @@
       <c r="F137" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G137" s="19" t="s">
+      <c r="G137" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B138" s="11" t="s">
+      <c r="B138" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C138" s="12" t="s">
+      <c r="C138" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="D138" s="17" t="s">
+      <c r="D138" s="15" t="s">
         <v>408</v>
       </c>
       <c r="E138" s="1" t="s">
@@ -5368,18 +5381,18 @@
       <c r="F138" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G138" s="19" t="s">
+      <c r="G138" s="17" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B139" s="11" t="s">
+      <c r="B139" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C139" s="12" t="s">
+      <c r="C139" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="D139" s="17" t="s">
+      <c r="D139" s="15" t="s">
         <v>412</v>
       </c>
       <c r="E139" s="1" t="s">
@@ -5388,18 +5401,18 @@
       <c r="F139" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="G139" s="19" t="s">
+      <c r="G139" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B140" s="11" t="s">
+      <c r="B140" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C140" s="12" t="s">
+      <c r="C140" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="D140" s="17" t="s">
+      <c r="D140" s="15" t="s">
         <v>415</v>
       </c>
       <c r="E140" s="1" t="s">
@@ -5408,18 +5421,18 @@
       <c r="F140" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G140" s="19" t="s">
+      <c r="G140" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="141" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B141" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C141" s="12" t="s">
+      <c r="B141" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="D141" s="17" t="s">
+      <c r="D141" s="15" t="s">
         <v>417</v>
       </c>
       <c r="E141" s="1" t="s">
@@ -5428,18 +5441,18 @@
       <c r="F141" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G141" s="19" t="s">
+      <c r="G141" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B142" s="11" t="s">
+      <c r="B142" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C142" s="12" t="s">
+      <c r="C142" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="D142" s="17" t="s">
+      <c r="D142" s="15" t="s">
         <v>419</v>
       </c>
       <c r="E142" s="1" t="s">
@@ -5448,18 +5461,18 @@
       <c r="F142" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G142" s="19" t="s">
+      <c r="G142" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="11" t="s">
+      <c r="B143" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C143" s="12" t="s">
+      <c r="C143" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="D143" s="17" t="s">
+      <c r="D143" s="15" t="s">
         <v>356</v>
       </c>
       <c r="E143" s="1" t="s">
@@ -5468,18 +5481,18 @@
       <c r="F143" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="G143" s="19" t="s">
+      <c r="G143" s="17" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B144" s="11" t="s">
+      <c r="B144" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C144" s="12" t="s">
+      <c r="C144" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="D144" s="17" t="s">
+      <c r="D144" s="15" t="s">
         <v>424</v>
       </c>
       <c r="E144" s="1" t="s">
@@ -5488,18 +5501,18 @@
       <c r="F144" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G144" s="19" t="s">
+      <c r="G144" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B145" s="11" t="s">
+      <c r="B145" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C145" s="12" t="s">
+      <c r="C145" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="D145" s="17" t="s">
+      <c r="D145" s="15" t="s">
         <v>426</v>
       </c>
       <c r="E145" s="1" t="s">
@@ -5508,16 +5521,16 @@
       <c r="F145" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G145" s="19"/>
+      <c r="G145" s="17"/>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B146" s="11" t="s">
+      <c r="B146" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C146" s="12" t="s">
+      <c r="C146" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="D146" s="17" t="s">
+      <c r="D146" s="15" t="s">
         <v>428</v>
       </c>
       <c r="E146" s="1" t="s">
@@ -5526,18 +5539,18 @@
       <c r="F146" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G146" s="19" t="s">
+      <c r="G146" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B147" s="11" t="s">
+      <c r="B147" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C147" s="12" t="s">
+      <c r="C147" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="D147" s="17" t="s">
+      <c r="D147" s="15" t="s">
         <v>356</v>
       </c>
       <c r="E147" s="1" t="s">
@@ -5546,18 +5559,18 @@
       <c r="F147" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G147" s="19" t="s">
+      <c r="G147" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C148" s="12" t="s">
+      <c r="C148" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="D148" s="17" t="s">
+      <c r="D148" s="15" t="s">
         <v>431</v>
       </c>
       <c r="E148" s="1" t="s">
@@ -5566,18 +5579,18 @@
       <c r="F148" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G148" s="19" t="s">
+      <c r="G148" s="17" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C149" s="12" t="s">
+      <c r="C149" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="D149" s="17" t="s">
+      <c r="D149" s="15" t="s">
         <v>433</v>
       </c>
       <c r="E149" s="1" t="s">
@@ -5586,16 +5599,16 @@
       <c r="F149" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G149" s="19"/>
+      <c r="G149" s="17"/>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C150" s="12" t="s">
+      <c r="C150" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="D150" s="17" t="s">
+      <c r="D150" s="15" t="s">
         <v>436</v>
       </c>
       <c r="E150" s="1" t="s">
@@ -5604,18 +5617,18 @@
       <c r="F150" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="G150" s="19" t="s">
+      <c r="G150" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B151" s="11" t="s">
+      <c r="B151" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C151" s="12" t="s">
+      <c r="C151" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="D151" s="17" t="s">
+      <c r="D151" s="15" t="s">
         <v>438</v>
       </c>
       <c r="E151" s="1" t="s">
@@ -5624,18 +5637,18 @@
       <c r="F151" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G151" s="19" t="s">
+      <c r="G151" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B152" s="11" t="s">
+      <c r="B152" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C152" s="12" t="s">
+      <c r="C152" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="D152" s="17" t="s">
+      <c r="D152" s="15" t="s">
         <v>441</v>
       </c>
       <c r="E152" s="1" t="s">
@@ -5644,16 +5657,16 @@
       <c r="F152" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G152" s="19"/>
+      <c r="G152" s="17"/>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B153" s="11" t="s">
+      <c r="B153" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C153" s="12" t="s">
+      <c r="C153" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="D153" s="17" t="s">
+      <c r="D153" s="15" t="s">
         <v>443</v>
       </c>
       <c r="E153" s="1" t="s">
@@ -5662,18 +5675,18 @@
       <c r="F153" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="G153" s="19" t="s">
+      <c r="G153" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C154" s="12" t="s">
+      <c r="C154" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="D154" s="17" t="s">
+      <c r="D154" s="15" t="s">
         <v>446</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -5682,18 +5695,18 @@
       <c r="F154" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G154" s="19" t="s">
+      <c r="G154" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C155" s="12" t="s">
+      <c r="B155" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="D155" s="17" t="s">
+      <c r="D155" s="15" t="s">
         <v>448</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -5702,18 +5715,18 @@
       <c r="F155" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="G155" s="19" t="s">
+      <c r="G155" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B156" s="11" t="s">
+      <c r="B156" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C156" s="12" t="s">
+      <c r="C156" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="D156" s="17" t="s">
+      <c r="D156" s="15" t="s">
         <v>451</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -5722,18 +5735,18 @@
       <c r="F156" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="G156" s="19" t="s">
+      <c r="G156" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B157" s="11" t="s">
+      <c r="B157" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C157" s="12" t="s">
+      <c r="C157" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D157" s="17" t="s">
+      <c r="D157" s="15" t="s">
         <v>454</v>
       </c>
       <c r="E157" s="1" t="s">
@@ -5742,18 +5755,18 @@
       <c r="F157" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="G157" s="19" t="s">
+      <c r="G157" s="17" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B158" s="11" t="s">
+      <c r="B158" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C158" s="12" t="s">
+      <c r="C158" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="D158" s="17" t="s">
+      <c r="D158" s="15" t="s">
         <v>458</v>
       </c>
       <c r="E158" s="1" t="s">
@@ -5762,18 +5775,18 @@
       <c r="F158" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G158" s="19" t="s">
+      <c r="G158" s="17" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B159" s="11" t="s">
+      <c r="B159" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C159" s="12" t="s">
+      <c r="C159" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="D159" s="17" t="s">
+      <c r="D159" s="15" t="s">
         <v>460</v>
       </c>
       <c r="E159" s="1" t="s">
@@ -5782,18 +5795,18 @@
       <c r="F159" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="G159" s="19" t="s">
+      <c r="G159" s="17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B160" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C160" s="12" t="s">
+      <c r="B160" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="D160" s="17" t="s">
+      <c r="D160" s="15" t="s">
         <v>463</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -5802,18 +5815,18 @@
       <c r="F160" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G160" s="19" t="s">
+      <c r="G160" s="17" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="161" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B161" s="11" t="s">
+      <c r="B161" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C161" s="12" t="s">
+      <c r="C161" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D161" s="17" t="s">
+      <c r="D161" s="15" t="s">
         <v>467</v>
       </c>
       <c r="E161" s="1" t="s">
@@ -5822,18 +5835,18 @@
       <c r="F161" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="G161" s="19" t="s">
+      <c r="G161" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C162" s="12" t="s">
+      <c r="B162" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="D162" s="17" t="s">
+      <c r="D162" s="15" t="s">
         <v>470</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -5842,16 +5855,16 @@
       <c r="F162" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G162" s="19"/>
+      <c r="G162" s="17"/>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B163" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" s="12" t="s">
+      <c r="B163" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C163" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="D163" s="17" t="s">
+      <c r="D163" s="15" t="s">
         <v>472</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -5860,18 +5873,18 @@
       <c r="F163" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G163" s="19" t="s">
+      <c r="G163" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B164" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C164" s="12" t="s">
+      <c r="B164" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="D164" s="17" t="s">
+      <c r="D164" s="15" t="s">
         <v>474</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -5880,18 +5893,18 @@
       <c r="F164" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G164" s="19" t="s">
+      <c r="G164" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B165" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C165" s="12" t="s">
+      <c r="B165" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="D165" s="17" t="s">
+      <c r="D165" s="15" t="s">
         <v>476</v>
       </c>
       <c r="E165" s="1" t="s">
@@ -5900,18 +5913,18 @@
       <c r="F165" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G165" s="19" t="s">
+      <c r="G165" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="166" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B166" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C166" s="12" t="s">
+      <c r="B166" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="D166" s="17" t="s">
+      <c r="D166" s="15" t="s">
         <v>478</v>
       </c>
       <c r="E166" s="1" t="s">
@@ -5920,18 +5933,18 @@
       <c r="F166" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G166" s="19" t="s">
+      <c r="G166" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="167" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B167" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" s="12" t="s">
+      <c r="B167" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="D167" s="17" t="s">
+      <c r="D167" s="15" t="s">
         <v>480</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -5940,18 +5953,18 @@
       <c r="F167" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G167" s="19" t="s">
+      <c r="G167" s="17" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B168" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="12" t="s">
+      <c r="B168" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D168" s="17" t="s">
+      <c r="D168" s="15" t="s">
         <v>485</v>
       </c>
       <c r="E168" s="1" t="s">
@@ -5960,25 +5973,25 @@
       <c r="F168" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="G168" s="19"/>
+      <c r="G168" s="17"/>
     </row>
     <row r="169" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C169" s="14" t="s">
+      <c r="B169" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="D169" s="18" t="s">
+      <c r="D169" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="E169" s="15" t="s">
+      <c r="E169" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F169" s="15" t="s">
+      <c r="F169" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="G169" s="20"/>
+      <c r="G169" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>